<commit_message>
Popravljen scenarij registracije korisnika
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/ScenarijRegistracijeKorisnika.xlsx
+++ b/UseCaseIScenarij/ScenarijRegistracijeKorisnika.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belma\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belma\Desktop\SL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -25,11 +26,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Scenarij 1 - Registracija online korisnika</t>
   </si>
   <si>
+    <t>Online korisnik</t>
+  </si>
+  <si>
+    <t>Alternativni tok 1</t>
+  </si>
+  <si>
+    <t>Alternativni tok 2</t>
+  </si>
+  <si>
+    <t>1. Odabir putovanja</t>
+  </si>
+  <si>
+    <t>2. Provjera slobodnih mjesta</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -39,121 +55,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Glavni tok: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Online korisnik kreira račun i bira putovanje</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Preduvjeti: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Da bi odabrao i uplatio putovanje, korisnik mora imati kreiran račun na stranici </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TravelBook-a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Posljedice: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ukoliko korisnik odustane od putovanja, gubi određeni postotak cijene putovanja, koji je unaprijed određen kao osiguranje.</t>
-    </r>
-  </si>
-  <si>
-    <t>Online korisnik</t>
-  </si>
-  <si>
-    <t>TravelBook</t>
-  </si>
-  <si>
-    <t>1. Popunjavanje podataka</t>
-  </si>
-  <si>
-    <t>2. Autorizacija podataka</t>
-  </si>
-  <si>
-    <t>3. Kreiranje korisničkog računa</t>
-  </si>
-  <si>
-    <t>4. Pristup kreiranim putovanjima</t>
-  </si>
-  <si>
-    <t>Alternativni tok 1</t>
-  </si>
-  <si>
-    <t>Za korak 2 : Autorizacija podataka</t>
-  </si>
-  <si>
-    <t>2. Uspješna registracija, prelazak na korak 3.</t>
-  </si>
-  <si>
-    <t>1. Postoji već identičan e-mail korisnika u bazi podataka</t>
-  </si>
-  <si>
-    <t>Alternativni tok 2</t>
-  </si>
-  <si>
-    <t>Za korak 4: Uplata putovanja</t>
-  </si>
-  <si>
-    <t>1. Odabir putovanja</t>
-  </si>
-  <si>
-    <t>2. Provjera slobodnih mjesta</t>
-  </si>
-  <si>
-    <t>3. Broj putnika već popunjen, obavještava se korisnik</t>
-  </si>
-  <si>
-    <t>4. Postoje slobodna mjesta</t>
-  </si>
-  <si>
-    <t>5. Rezervacija i uplata putovanja</t>
-  </si>
-  <si>
-    <t>6. Odobrenje rezervacije i uplate putovanja</t>
+      <t>Naziv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:  Registracija online korisnika na stranicu</t>
+    </r>
   </si>
   <si>
     <r>
@@ -177,13 +90,24 @@
       </rPr>
       <t xml:space="preserve"> Ukoliko klijent želi da kupi kartu za određeno putovanje online, preko TravelBook-a, prvo se mora registrovati na stranicu. 
 Registracija se sastoji od unosa ličnih podataka (ime, prezime, datum rođenja, JMBG, kontakt telefon, adresa stanovanja, podataka o kreditnoj kartici, e-mail adres i password). 
-Nakon provjere unesenih podataka, ako je sve uspješno odrađeno (e-mail adresa nije već registrovana), kreira se profil korisnika u bazi podataka  TravelBook-a.
-Poslije registracije, korisnik će imati mogućnost pregleda svih ponuđenih putovanja od strane turističkih agencija, 
-te odabrati, rezervisati i uplatiti neko putovanje, ukoliko to želi.
-</t>
-    </r>
-  </si>
-  <si>
+Nakon provjere unesenih podataka, ako je sve uspješno odrađeno (e-mail adresa nije već registrovana), kreira se profil korisnika u bazi podataka  TravelBook-a. Poslije registracije, korisnik će imati mogućnost pregleda svih ponuđenih putovanja od strane turističkih agencija, 
+te odabrati, rezervisati i uplatiti neko putovanje, ukoliko to želi.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Preduvjeti: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Da bi odabrao i uplatio putovanje, korisnik mora imati kreiran račun na stranici </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -193,25 +117,170 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Naziv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:  Registracija online korisnika na stranicu</t>
-    </r>
+      <t xml:space="preserve">TravelBook-a, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kreditnu karticu preko koje će platiti putovanje i internet konekciju.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Posljedice: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Jednostavno kreiranje korisničkog računa, na stranici </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TravelBook-a, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>radi pretraživanja i uplaćivanja putovanja.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Glavni tok: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Online korisnik kreira račun i bira putovanje.</t>
+    </r>
+  </si>
+  <si>
+    <t>TravelBook administrator</t>
+  </si>
+  <si>
+    <t>1. Unos imena korisnika</t>
+  </si>
+  <si>
+    <t>2. Unos prezimena</t>
+  </si>
+  <si>
+    <t>3. Unos datuma rođenja</t>
+  </si>
+  <si>
+    <t>4. Unos JMBG-a</t>
+  </si>
+  <si>
+    <t>5.Unos e-maila</t>
+  </si>
+  <si>
+    <t>6. Unos password-a</t>
+  </si>
+  <si>
+    <t>7. Unos adrese stanovanje</t>
+  </si>
+  <si>
+    <t>8. Unos kontakt telefona</t>
+  </si>
+  <si>
+    <t>9. Unos podataka o kreditnoj kartici</t>
+  </si>
+  <si>
+    <t>10.  Autorizacija podataka</t>
+  </si>
+  <si>
+    <t>11. Kreiranje korisničkog računa</t>
+  </si>
+  <si>
+    <t>12. Pristup kreiranim putovanjima</t>
+  </si>
+  <si>
+    <t>1. Uspješna registracija</t>
+  </si>
+  <si>
+    <t>2.  Unesene podaci su validni</t>
+  </si>
+  <si>
+    <t>3. Potvrda o uspješno kreiranom računu</t>
+  </si>
+  <si>
+    <t>3. Postoje slobodna mjesta</t>
+  </si>
+  <si>
+    <t>4. Rezervacija i uplata putovanja</t>
+  </si>
+  <si>
+    <t>5. Odobrenje rezervacije i uplate putovanja</t>
+  </si>
+  <si>
+    <t>Alternativni tok 3</t>
+  </si>
+  <si>
+    <t>Za korak 10 : Uspješna autorizacija podataka</t>
+  </si>
+  <si>
+    <t>Za korak 12: Uspješna uplata putovanja</t>
+  </si>
+  <si>
+    <t>Za korak 10: Neuspjela autorizacija podataka</t>
+  </si>
+  <si>
+    <t>1.  Neuspjela registracija</t>
+  </si>
+  <si>
+    <t>2. E-mail već postoji za drugi korisnički račun</t>
+  </si>
+  <si>
+    <t>3. JMBG isti kao kod drugog korisnika</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,13 +292,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,12 +317,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -280,35 +350,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:C12" totalsRowShown="0">
-  <autoFilter ref="B9:C12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:C21" totalsRowShown="0">
+  <autoFilter ref="B9:C21"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Online korisnik"/>
-    <tableColumn id="2" name="TravelBook"/>
+    <tableColumn id="2" name="TravelBook administrator"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B16:C18" totalsRowShown="0">
-  <autoFilter ref="B16:C18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B26:C28" totalsRowShown="0">
+  <autoFilter ref="B26:C28"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Online korisnik"/>
-    <tableColumn id="2" name="TravelBook"/>
+    <tableColumn id="2" name="TravelBook administrator"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B24:C28" totalsRowShown="0">
-  <autoFilter ref="B24:C28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B34:C37" totalsRowShown="0">
+  <autoFilter ref="B34:C37"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Online korisnik"/>
-    <tableColumn id="2" name="TravelBook"/>
+    <tableColumn id="2" name="TravelBook administrator"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B43:C45" totalsRowShown="0">
+  <autoFilter ref="B43:C45"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Online korisnik"/>
+    <tableColumn id="2" name="TravelBook administrator"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -609,10 +690,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,139 +716,243 @@
     <col min="3" max="3" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="345" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="22" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C26" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="43" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>21</v>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B24:C24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>